<commit_message>
modified mac directory. updated code to match directory changes. made some progress on filtering data. used xlookup to retrieve movie info from movies dataset.
</commit_message>
<xml_diff>
--- a/movie-release-optimization/data/output/xlsx/filtered_movies.xlsx
+++ b/movie-release-optimization/data/output/xlsx/filtered_movies.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kitkat/github projects/Marvel-Analytics-by-KS/movie-release-optimization/data/output/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FFB87555-1FBD-7F43-8E5A-71668DEC21FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8504CB-E3B6-B448-A973-E963F44B9FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="80" windowWidth="28040" windowHeight="17180" xr2:uid="{2A2474E0-C2C1-0B4A-BABD-00CFE353F286}"/>
+    <workbookView xWindow="19180" yWindow="0" windowWidth="19220" windowHeight="21600" xr2:uid="{2A2474E0-C2C1-0B4A-BABD-00CFE353F286}"/>
   </bookViews>
   <sheets>
     <sheet name="filtered_movies" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -6489,7 +6502,7 @@
   <dimension ref="A1:C1812"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>